<commit_message>
added sensitivity and made changes in outputs
</commit_message>
<xml_diff>
--- a/output/Baseline/baseline-arr10-mm1-res.xlsx
+++ b/output/Baseline/baseline-arr10-mm1-res.xlsx
@@ -15,18 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
   <si>
     <t>stat</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>Stage_1/2</t>
-  </si>
-  <si>
-    <t>Stage_3/4</t>
+    <t>no_cancer</t>
+  </si>
+  <si>
+    <t>cancer</t>
+  </si>
+  <si>
+    <t>stage_1_2</t>
+  </si>
+  <si>
+    <t>stage_3_4</t>
   </si>
   <si>
     <t>1</t>
@@ -44,82 +47,49 @@
     <t>5</t>
   </si>
   <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>unique_arrivals</t>
+  </si>
+  <si>
+    <t>total_scanned</t>
+  </si>
+  <si>
+    <t>total_returns</t>
+  </si>
+  <si>
+    <t>effective_arr_rate</t>
+  </si>
+  <si>
+    <t>Wait Time</t>
+  </si>
+  <si>
+    <t>Time in System</t>
+  </si>
+  <si>
+    <t>Service Time</t>
+  </si>
+  <si>
+    <t>Queue Size</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
     <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>median</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>Percentage of Total Scans</t>
-  </si>
-  <si>
-    <t>Pecentage of all Cancer Results</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>unique_arrivals</t>
-  </si>
-  <si>
-    <t>total_scanned</t>
-  </si>
-  <si>
-    <t>total_returns</t>
-  </si>
-  <si>
-    <t>Wait Time</t>
-  </si>
-  <si>
-    <t>Time in System</t>
-  </si>
-  <si>
-    <t>Service Time</t>
-  </si>
-  <si>
-    <t>Queue Size</t>
   </si>
   <si>
     <t>avg_max</t>
@@ -199,260 +169,108 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>22499.666666666668</v>
       </c>
       <c r="D2" t="n">
+        <v>1878.1666666666667</v>
+      </c>
+      <c r="E2" t="n">
         <v>1318.2</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>559.9666666666667</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>223.93061322702147</v>
       </c>
       <c r="D3" t="n">
+        <v>48.772578031267656</v>
+      </c>
+      <c r="E3" t="n">
         <v>36.93554497714391</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>24.885230813550397</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="C4" t="n">
+        <v>22554.5</v>
       </c>
       <c r="D4" t="n">
+        <v>1871.0</v>
+      </c>
+      <c r="E4" t="n">
         <v>1320.0</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>560.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="C5" t="n">
+        <v>23072.0</v>
       </c>
       <c r="D5" t="n">
+        <v>1988.0</v>
+      </c>
+      <c r="E5" t="n">
         <v>1397.0</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>606.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="C6" t="n">
+        <v>21870.0</v>
       </c>
       <c r="D6" t="n">
+        <v>1792.0</v>
+      </c>
+      <c r="E6" t="n">
         <v>1244.0</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>490.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5.407367455547812</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2.296882625515369</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.14118830184115785</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.0959387341364561</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="n">
-        <v>5.406573974639301</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2.3081006095091094</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="n">
-        <v>5.68764758570149</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2.4665228540030117</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5.1515653470266685</v>
-      </c>
-      <c r="E11" t="n">
-        <v>2.0130643769771166</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="n">
-        <v>70.18851335706991</v>
-      </c>
-      <c r="E12" t="n">
-        <v>29.81148664293009</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9981805967411896</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.9981805967411886</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="n">
-        <v>70.12774608268458</v>
-      </c>
-      <c r="E14" t="n">
-        <v>29.872253917315426</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="n">
-        <v>72.65625</v>
-      </c>
-      <c r="E15" t="n">
-        <v>31.796246648793563</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" t="n">
-        <v>68.20375335120643</v>
-      </c>
-      <c r="E16" t="n">
-        <v>27.34375</v>
       </c>
     </row>
   </sheetData>
@@ -471,24 +289,27 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>16602.166666666668</v>
@@ -499,13 +320,16 @@
       <c r="E2" t="n">
         <v>10653.433333333332</v>
       </c>
+      <c r="F2" t="n">
+        <v>25.236666666666668</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
         <v>139.7177162348607</v>
@@ -516,13 +340,16 @@
       <c r="E3" t="n">
         <v>130.2752214864106</v>
       </c>
+      <c r="F3" t="n">
+        <v>0.1714060433356215</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
         <v>16618.5</v>
@@ -533,13 +360,16 @@
       <c r="E4" t="n">
         <v>10652.0</v>
       </c>
+      <c r="F4" t="n">
+        <v>25.252314814814817</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C5" t="n">
         <v>16920.0</v>
@@ -550,13 +380,16 @@
       <c r="E5" t="n">
         <v>10965.0</v>
       </c>
+      <c r="F5" t="n">
+        <v>25.57777777777778</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
         <v>16277.0</v>
@@ -566,6 +399,9 @@
       </c>
       <c r="E6" t="n">
         <v>10206.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>24.812962962962963</v>
       </c>
     </row>
   </sheetData>
@@ -587,24 +423,24 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>80.52231065240079</v>
@@ -621,10 +457,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
         <v>6.779448159402665</v>
@@ -641,10 +477,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
         <v>79.45392499999997</v>
@@ -661,10 +497,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n">
         <v>115.24377</v>
@@ -681,10 +517,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C6" t="n">
         <v>44.078719999999976</v>
@@ -701,10 +537,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C7" t="n">
         <v>129.85159999999973</v>
@@ -721,10 +557,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C8" t="n">
         <v>33.61909999999989</v>
@@ -758,84 +594,84 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>103.06661600694123</v>
+        <v>34.35553866898041</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>0.09579958318198173</v>
+        <v>0.03193319439399357</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>102.150000000006</v>
+        <v>34.050000000002</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" t="n">
-        <v>122.65999999999622</v>
+        <v>40.886666666665406</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C6" t="n">
-        <v>60.168999999998505</v>
+        <v>20.056333333332834</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C7" t="n">
-        <v>128.33999999998014</v>
+        <v>42.77999999999338</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C8" t="n">
-        <v>9.959999999955471</v>
+        <v>3.319999999985157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>